<commit_message>
created user_validation, income & generate_data tests funtiuons
</commit_message>
<xml_diff>
--- a/output/expenses_record.xlsx
+++ b/output/expenses_record.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D122"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,40 +458,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2022-01-02</t>
+          <t>2022-01-01</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>326.15</v>
+        <v>270.99</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2022-01-07</t>
+          <t>2022-01-04</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>293.13</v>
+        <v>373.64</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
@@ -503,75 +503,75 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2022-01-12</t>
+          <t>2022-01-20</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>14.4</v>
+        <v>195.88</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2022-01-14</t>
+          <t>2022-01-28</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>152.58</v>
+        <v>251.89</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2022-01-16</t>
+          <t>2022-01-29</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>51.01</v>
+        <v>268.35</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2022-01-20</t>
+          <t>2022-02-01</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>50.27</v>
+        <v>337.72</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
@@ -583,211 +583,211 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2022-01-26</t>
+          <t>2022-02-04</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>365.48</v>
+        <v>79.38</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2022-01-27</t>
+          <t>2022-02-09</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>15.38</v>
+        <v>281.03</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2022-02-02</t>
+          <t>2022-02-17</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>303.81</v>
+        <v>130.87</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Pet</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2022-02-05</t>
+          <t>2022-02-20</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>120</v>
+        <v>433.15</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2022-02-05</t>
+          <t>2022-02-20</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>306.06</v>
+        <v>66.04000000000001</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2022-02-07</t>
+          <t>2022-03-01</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>217.98</v>
+        <v>396.19</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2022-02-18</t>
+          <t>2022-03-01</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>353.45</v>
+        <v>59.78</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2022-02-19</t>
+          <t>2022-03-07</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>323.32</v>
+        <v>15.5</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2022-02-20</t>
+          <t>2022-03-09</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>39.01</v>
+        <v>317.12</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2022-02-27</t>
+          <t>2022-03-11</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>269.34</v>
+        <v>237.88</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2022-03-01</t>
+          <t>2022-03-13</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>424.23</v>
+        <v>331.51</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -798,60 +798,60 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2022-03-04</t>
+          <t>2022-03-15</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>117.25</v>
+        <v>423.61</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-03-16</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>157.37</v>
+        <v>442.77</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2022-03-12</t>
+          <t>2022-03-17</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>125.89</v>
+        <v>251.3</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
@@ -863,55 +863,55 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2022-03-15</t>
+          <t>2022-03-20</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>123.52</v>
+        <v>409.4</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2022-03-16</t>
+          <t>2022-03-22</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>168.16</v>
+        <v>69.73999999999999</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2022-03-20</t>
+          <t>2022-03-25</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>68.95999999999999</v>
+        <v>277.01</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
@@ -923,135 +923,135 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2022-03-21</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>127.57</v>
+        <v>382.49</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2022-03-22</t>
+          <t>2022-04-01</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>268.55</v>
+        <v>309.63</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2022-03-31</t>
+          <t>2022-04-05</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>83.72</v>
+        <v>268.37</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2022-03-31</t>
+          <t>2022-04-06</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>417.75</v>
+        <v>263.57</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2022-04-04</t>
+          <t>2022-04-09</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>84.73999999999999</v>
+        <v>242.9</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2022-04-05</t>
+          <t>2022-04-09</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>216.77</v>
+        <v>410.68</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2022-04-11</t>
+          <t>2022-04-17</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>186.82</v>
+        <v>336.61</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>party</t>
         </is>
       </c>
     </row>
@@ -1063,195 +1063,195 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2022-04-14</t>
+          <t>2022-04-21</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>60.2</v>
+        <v>378</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2022-04-17</t>
+          <t>2022-04-27</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>219.89</v>
+        <v>184.17</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2022-04-18</t>
+          <t>2022-04-27</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>383.99</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2022-04-19</t>
+          <t>2022-04-27</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>31.12</v>
+        <v>17.52</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2022-04-20</t>
+          <t>2022-04-28</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>28.92</v>
+        <v>437.86</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2022-04-22</t>
+          <t>2022-04-29</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>383.16</v>
+        <v>433.29</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2022-04-24</t>
+          <t>2022-05-01</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>46.74</v>
+        <v>421.82</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2022-04-28</t>
+          <t>2022-05-03</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>337.86</v>
+        <v>319.91</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2022-04-29</t>
+          <t>2022-05-07</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>349.85</v>
+        <v>378.36</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2022-04-29</t>
+          <t>2022-05-13</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>221.27</v>
+        <v>35.22</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
@@ -1263,11 +1263,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2022-05-01</t>
+          <t>2022-05-14</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>128.83</v>
+        <v>152.28</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1283,35 +1283,35 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2022-05-07</t>
+          <t>2022-05-16</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>87.78</v>
+        <v>161.84</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-19</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>356.1</v>
+        <v>163.11</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
@@ -1323,31 +1323,31 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-20</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>25.56</v>
+        <v>19.1</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2022-05-14</t>
+          <t>2022-05-22</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>43.68</v>
+        <v>339.44</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1358,60 +1358,60 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2022-05-15</t>
+          <t>2022-05-23</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>262.11</v>
+        <v>79.14</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2022-05-19</t>
+          <t>2022-05-26</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>423.4</v>
+        <v>85.04000000000001</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2022-05-20</t>
+          <t>2022-06-04</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>188.55</v>
+        <v>97.47</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
@@ -1423,55 +1423,55 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2022-05-24</t>
+          <t>2022-06-05</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>253.46</v>
+        <v>299.09</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2022-05-25</t>
+          <t>2022-06-07</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>68.54000000000001</v>
+        <v>353.8</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2022-05-26</t>
+          <t>2022-06-09</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>347.47</v>
+        <v>406.21</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
@@ -1483,71 +1483,71 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2022-05-27</t>
+          <t>2022-06-10</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>410.77</v>
+        <v>172.51</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2022-05-27</t>
+          <t>2022-06-12</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>327.86</v>
+        <v>357.51</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2022-05-29</t>
+          <t>2022-06-14</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>415.25</v>
+        <v>391.47</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2022-05-31</t>
+          <t>2022-06-14</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>96.7</v>
+        <v>348.05</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1558,56 +1558,56 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2022-06-06</t>
+          <t>2022-06-20</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>6.55</v>
+        <v>188.55</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2022-06-11</t>
+          <t>2022-06-29</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>443.39</v>
+        <v>351.12</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2022-06-16</t>
+          <t>2022-06-30</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>77.20999999999999</v>
+        <v>241.79</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1618,40 +1618,40 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2022-06-17</t>
+          <t>2022-06-30</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>30.25</v>
+        <v>93.95999999999999</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2022-06-22</t>
+          <t>2022-07-05</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>224.19</v>
+        <v>43.23</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
@@ -1663,15 +1663,15 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2022-06-23</t>
+          <t>2022-07-06</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>257.95</v>
+        <v>81.79000000000001</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
@@ -1683,31 +1683,31 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2022-06-24</t>
+          <t>2022-07-06</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>21.08</v>
+        <v>407.99</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2022-06-25</t>
+          <t>2022-07-07</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>103</v>
+        <v>345.48</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -1718,20 +1718,20 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2022-06-26</t>
+          <t>2022-07-09</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>387.16</v>
+        <v>287.44</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
@@ -1743,35 +1743,35 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2022-06-26</t>
+          <t>2022-07-09</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>345.83</v>
+        <v>380.51</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2022-06-27</t>
+          <t>2022-07-14</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>37.07</v>
+        <v>343.09</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
@@ -1783,31 +1783,31 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2022-06-28</t>
+          <t>2022-07-15</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>227.39</v>
+        <v>20.66</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2022-07-02</t>
+          <t>2022-07-20</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>298.5</v>
+        <v>447.28</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -1818,100 +1818,100 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2022-07-03</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>371.5</v>
+        <v>55.44</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2022-07-06</t>
+          <t>2022-07-26</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>183.26</v>
+        <v>232.11</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2022-07-07</t>
+          <t>2022-07-28</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>101.3</v>
+        <v>311.96</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2022-07-07</t>
+          <t>2022-07-29</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>170.58</v>
+        <v>382.81</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2022-07-12</t>
+          <t>2022-08-01</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>204.65</v>
+        <v>36.04</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
@@ -1923,55 +1923,55 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2022-07-21</t>
+          <t>2022-08-07</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>67.55</v>
+        <v>341.8</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2022-07-23</t>
+          <t>2022-08-08</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>239.92</v>
+        <v>194.93</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-08-08</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>379.1</v>
+        <v>299.16</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
@@ -1983,11 +1983,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2022-07-27</t>
+          <t>2022-08-08</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>116.35</v>
+        <v>56.39</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -1998,76 +1998,76 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2022-08-03</t>
+          <t>2022-08-13</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>11.39</v>
+        <v>122.98</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2022-08-04</t>
+          <t>2022-08-19</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>75.05</v>
+        <v>78.93000000000001</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2022-08-04</t>
+          <t>2022-08-19</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>273.9</v>
+        <v>205.29</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2022-08-04</t>
+          <t>2022-08-20</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>296.09</v>
+        <v>138.59</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2078,36 +2078,36 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2022-08-11</t>
+          <t>2022-08-25</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>188.36</v>
+        <v>94.87</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2022-08-17</t>
+          <t>2022-08-28</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>273.18</v>
+        <v>2.32</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2118,16 +2118,16 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2022-08-17</t>
+          <t>2022-09-04</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>97.8</v>
+        <v>129.9</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2138,36 +2138,36 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2022-08-24</t>
+          <t>2022-09-06</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>40.46</v>
+        <v>445.71</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2022-08-25</t>
+          <t>2022-09-09</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>175.05</v>
+        <v>63.26</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2178,27 +2178,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2022-09-04</t>
+          <t>2022-09-11</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>104.74</v>
+        <v>253.08</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2207,11 +2207,11 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>293.89</v>
+        <v>228.64</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
@@ -2223,51 +2223,51 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2022-09-16</t>
+          <t>2022-09-15</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>235.5</v>
+        <v>284.69</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2022-09-17</t>
+          <t>2022-09-21</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>218</v>
+        <v>363.85</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2022-09-17</t>
+          <t>2022-09-25</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>64.94</v>
+        <v>445.02</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2278,40 +2278,40 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2022-09-17</t>
+          <t>2022-09-26</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>93.23</v>
+        <v>438.35</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2022-09-17</t>
+          <t>2022-10-02</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>342.5</v>
+        <v>285.24</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>party</t>
         </is>
       </c>
     </row>
@@ -2323,35 +2323,35 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2022-09-20</t>
+          <t>2022-10-04</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>370.3</v>
+        <v>197.08</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>2022-09-21</t>
+          <t>2022-10-06</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>148.82</v>
+        <v>288.72</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
@@ -2363,55 +2363,55 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>2022-09-25</t>
+          <t>2022-10-15</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>121.06</v>
+        <v>387.06</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2022-09-29</t>
+          <t>2022-10-17</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>159.21</v>
+        <v>2.75</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>2022-10-06</t>
+          <t>2022-10-18</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>147.78</v>
+        <v>283.61</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
@@ -2423,11 +2423,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>2022-10-09</t>
+          <t>2022-10-19</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>208.72</v>
+        <v>91.61</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -2438,20 +2438,20 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2022-10-10</t>
+          <t>2022-10-19</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>261.34</v>
+        <v>116.16</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>party</t>
         </is>
       </c>
     </row>
@@ -2463,55 +2463,55 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2022-10-11</t>
+          <t>2022-10-21</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>268.75</v>
+        <v>11.56</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>2022-10-12</t>
+          <t>2022-10-21</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>309.43</v>
+        <v>167.42</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2022-10-14</t>
+          <t>2022-11-01</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>104.86</v>
+        <v>113.17</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
@@ -2523,91 +2523,91 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>2022-10-21</t>
+          <t>2022-11-08</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>317.84</v>
+        <v>24.66</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>2022-10-24</t>
+          <t>2022-11-11</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>69.14</v>
+        <v>403.72</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>2022-10-29</t>
+          <t>2022-11-11</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>193.83</v>
+        <v>358.06</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2022-11-05</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>16.7</v>
+        <v>106.87</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>2022-11-05</t>
+          <t>2022-11-22</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>30.99</v>
+        <v>418.38</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -2618,76 +2618,76 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2022-11-10</t>
+          <t>2022-11-25</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>89.33</v>
+        <v>66.41</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>2022-11-11</t>
+          <t>2022-11-29</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>44.39</v>
+        <v>140.22</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2022-11-13</t>
+          <t>2022-12-03</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>232.46</v>
+        <v>152.13</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2022-11-15</t>
+          <t>2022-12-08</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>84.56</v>
+        <v>357.23</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -2698,140 +2698,140 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2022-11-17</t>
+          <t>2022-12-11</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>46.23</v>
+        <v>358.07</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2022-11-22</t>
+          <t>2022-12-16</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>153.88</v>
+        <v>374.19</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2022-11-25</t>
+          <t>2022-12-16</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>5.68</v>
+        <v>169.14</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>2022-11-25</t>
+          <t>2022-12-18</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>352.58</v>
+        <v>106.9</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2022-11-26</t>
+          <t>2022-12-18</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>89.75</v>
+        <v>304.98</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2022-11-26</t>
+          <t>2022-12-21</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>222.96</v>
+        <v>412.36</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>2022-12-13</t>
+          <t>2022-12-22</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>178.17</v>
+        <v>294.92</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
@@ -2843,35 +2843,15 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>2022-12-13</t>
+          <t>2022-12-28</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>21.38</v>
+        <v>120.71</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>insurance</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>Jonny Udoh</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>2022-12-31</t>
-        </is>
-      </c>
-      <c r="C122" t="n">
-        <v>150.92</v>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>grocery</t>
+          <t>party</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added remaining test functions
</commit_message>
<xml_diff>
--- a/output/expenses_record.xlsx
+++ b/output/expenses_record.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,56 +458,56 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2022-01-01</t>
+          <t>2022-01-03</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>270.99</v>
+        <v>407.75</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2022-01-04</t>
+          <t>2022-01-05</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>373.64</v>
+        <v>349.32</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2022-01-20</t>
+          <t>2022-01-05</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>195.88</v>
+        <v>111.63</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -518,136 +518,136 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2022-01-28</t>
+          <t>2022-01-07</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>251.89</v>
+        <v>186.01</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2022-01-29</t>
+          <t>2022-01-10</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>268.35</v>
+        <v>260.7</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2022-02-01</t>
+          <t>2022-01-10</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>337.72</v>
+        <v>315.29</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2022-02-04</t>
+          <t>2022-01-11</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>79.38</v>
+        <v>104.59</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2022-02-09</t>
+          <t>2022-01-14</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>281.03</v>
+        <v>253.6</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2022-02-17</t>
+          <t>2022-01-15</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>130.87</v>
+        <v>383.26</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2022-02-20</t>
+          <t>2022-01-16</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>433.15</v>
+        <v>376.66</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -658,16 +658,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2022-02-20</t>
+          <t>2022-01-19</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>66.04000000000001</v>
+        <v>43.62</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -678,56 +678,56 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2022-03-01</t>
+          <t>2022-01-20</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>396.19</v>
+        <v>376.09</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2022-03-01</t>
+          <t>2022-01-28</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>59.78</v>
+        <v>157.78</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2022-03-07</t>
+          <t>2022-01-28</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>15.5</v>
+        <v>275.34</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -738,20 +738,20 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2022-03-09</t>
+          <t>2022-01-29</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>317.12</v>
+        <v>407.97</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
@@ -763,71 +763,71 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2022-03-11</t>
+          <t>2022-02-01</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>237.88</v>
+        <v>252.21</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2022-03-13</t>
+          <t>2022-02-06</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>331.51</v>
+        <v>252.76</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2022-03-15</t>
+          <t>2022-02-16</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>423.61</v>
+        <v>187.77</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2022-03-16</t>
+          <t>2022-02-20</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>442.77</v>
+        <v>241.14</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -838,56 +838,56 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2022-03-17</t>
+          <t>2022-03-01</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>251.3</v>
+        <v>272.24</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2022-03-20</t>
+          <t>2022-03-04</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>409.4</v>
+        <v>396.56</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2022-03-22</t>
+          <t>2022-03-05</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>69.73999999999999</v>
+        <v>150.32</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -898,16 +898,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2022-03-25</t>
+          <t>2022-03-09</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>277.01</v>
+        <v>347.45</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -918,20 +918,20 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2022-03-13</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>382.49</v>
+        <v>258.44</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>party</t>
         </is>
       </c>
     </row>
@@ -943,31 +943,31 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2022-04-01</t>
+          <t>2022-03-16</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>309.63</v>
+        <v>47.83</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2022-04-05</t>
+          <t>2022-03-19</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>268.37</v>
+        <v>17.79</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -978,36 +978,36 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2022-04-06</t>
+          <t>2022-03-20</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>263.57</v>
+        <v>73.64</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2022-04-09</t>
+          <t>2022-03-23</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>242.9</v>
+        <v>232.42</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1018,56 +1018,56 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2022-04-09</t>
+          <t>2022-03-26</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>410.68</v>
+        <v>184.8</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2022-04-17</t>
+          <t>2022-03-30</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>336.61</v>
+        <v>322.3</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2022-04-21</t>
+          <t>2022-04-02</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>378</v>
+        <v>119.84</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1083,211 +1083,211 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2022-04-27</t>
+          <t>2022-04-02</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>184.17</v>
+        <v>238.28</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2022-04-27</t>
+          <t>2022-04-13</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>78.09999999999999</v>
+        <v>57.17</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2022-04-27</t>
+          <t>2022-04-14</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>17.52</v>
+        <v>321.34</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2022-04-28</t>
+          <t>2022-04-15</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>437.86</v>
+        <v>192.2</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2022-04-29</t>
+          <t>2022-04-23</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>433.29</v>
+        <v>304.25</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2022-05-01</t>
+          <t>2022-04-28</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>421.82</v>
+        <v>125.87</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2022-05-03</t>
+          <t>2022-04-29</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>319.91</v>
+        <v>200.91</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2022-05-07</t>
+          <t>2022-05-04</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>378.36</v>
+        <v>100.94</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2022-05-13</t>
+          <t>2022-05-05</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>35.22</v>
+        <v>418.16</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2022-05-14</t>
+          <t>2022-05-07</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>152.28</v>
+        <v>191.97</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2022-05-16</t>
+          <t>2022-05-08</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>161.84</v>
+        <v>342.34</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1298,36 +1298,36 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2022-05-19</t>
+          <t>2022-05-10</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>163.11</v>
+        <v>206.36</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2022-05-20</t>
+          <t>2022-05-11</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>19.1</v>
+        <v>45.26</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1338,60 +1338,60 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2022-05-22</t>
+          <t>2022-05-14</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>339.44</v>
+        <v>126.78</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2022-05-23</t>
+          <t>2022-05-15</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>79.14</v>
+        <v>66.16</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2022-05-26</t>
+          <t>2022-05-18</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>85.04000000000001</v>
+        <v>312.82</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
@@ -1403,11 +1403,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2022-06-04</t>
+          <t>2022-05-20</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>97.47</v>
+        <v>203.58</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1423,191 +1423,191 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2022-06-05</t>
+          <t>2022-05-25</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>299.09</v>
+        <v>129.07</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2022-06-07</t>
+          <t>2022-05-31</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>353.8</v>
+        <v>300.04</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2022-06-09</t>
+          <t>2022-05-31</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>406.21</v>
+        <v>384.74</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2022-06-10</t>
+          <t>2022-06-08</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>172.51</v>
+        <v>156.81</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2022-06-12</t>
+          <t>2022-06-10</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>357.51</v>
+        <v>272.27</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2022-06-14</t>
+          <t>2022-06-11</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>391.47</v>
+        <v>66.84999999999999</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2022-06-14</t>
+          <t>2022-06-12</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>348.05</v>
+        <v>164.71</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2022-06-20</t>
+          <t>2022-06-16</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>188.55</v>
+        <v>242.2</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2022-06-29</t>
+          <t>2022-06-16</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>351.12</v>
+        <v>248.79</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2022-06-30</t>
+          <t>2022-06-17</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>241.79</v>
+        <v>42.82</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1618,20 +1618,20 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2022-06-30</t>
+          <t>2022-06-20</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>93.95999999999999</v>
+        <v>417.41</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
@@ -1643,75 +1643,75 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2022-07-05</t>
+          <t>2022-06-24</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>43.23</v>
+        <v>135.79</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2022-07-06</t>
+          <t>2022-06-28</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>81.79000000000001</v>
+        <v>376.92</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2022-07-06</t>
+          <t>2022-07-05</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>407.99</v>
+        <v>357.13</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2022-07-07</t>
+          <t>2022-07-10</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>345.48</v>
+        <v>125.02</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
@@ -1723,91 +1723,91 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2022-07-09</t>
+          <t>2022-07-17</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>287.44</v>
+        <v>438.75</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2022-07-09</t>
+          <t>2022-07-19</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>380.51</v>
+        <v>110.89</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2022-07-14</t>
+          <t>2022-07-19</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>343.09</v>
+        <v>363.46</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2022-07-15</t>
+          <t>2022-07-24</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>20.66</v>
+        <v>310.57</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2022-07-20</t>
+          <t>2022-07-30</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>447.28</v>
+        <v>344.25</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -1818,180 +1818,180 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2022-07-25</t>
+          <t>2022-07-30</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>55.44</v>
+        <v>60.58</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-31</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>232.11</v>
+        <v>404.79</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2022-07-28</t>
+          <t>2022-08-01</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>311.96</v>
+        <v>375.73</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2022-07-29</t>
+          <t>2022-08-10</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>382.81</v>
+        <v>109.41</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2022-08-01</t>
+          <t>2022-08-13</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>36.04</v>
+        <v>410.97</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2022-08-07</t>
+          <t>2022-08-15</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>341.8</v>
+        <v>313.75</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2022-08-08</t>
+          <t>2022-08-17</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>194.93</v>
+        <v>39.96</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2022-08-08</t>
+          <t>2022-08-22</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>299.16</v>
+        <v>420.91</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2022-08-08</t>
+          <t>2022-08-23</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>56.39</v>
+        <v>15.82</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
@@ -2003,111 +2003,111 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2022-08-13</t>
+          <t>2022-08-24</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>122.98</v>
+        <v>154.29</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2022-08-19</t>
+          <t>2022-08-26</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>78.93000000000001</v>
+        <v>214.25</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2022-08-19</t>
+          <t>2022-08-26</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>205.29</v>
+        <v>165.85</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2022-08-20</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>138.59</v>
+        <v>19.88</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2022-08-25</t>
+          <t>2022-09-02</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>94.87</v>
+        <v>424.56</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2022-08-28</t>
+          <t>2022-09-03</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>2.32</v>
+        <v>232.49</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2118,76 +2118,76 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2022-09-04</t>
+          <t>2022-09-05</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>129.9</v>
+        <v>70.97</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2022-09-06</t>
+          <t>2022-09-08</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>445.71</v>
+        <v>159.76</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2022-09-09</t>
+          <t>2022-09-11</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>63.26</v>
+        <v>14.53</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2022-09-11</t>
+          <t>2022-09-13</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>253.08</v>
+        <v>87.02</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2198,76 +2198,76 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>2022-09-12</t>
+          <t>2022-09-14</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>228.64</v>
+        <v>18.6</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2022-09-15</t>
+          <t>2022-09-23</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>284.69</v>
+        <v>237.03</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2022-09-21</t>
+          <t>2022-09-29</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>363.85</v>
+        <v>258.75</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2022-09-25</t>
+          <t>2022-09-30</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>445.02</v>
+        <v>437.31</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2278,36 +2278,36 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2022-09-26</t>
+          <t>2022-10-02</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>438.35</v>
+        <v>190.37</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2022-10-02</t>
+          <t>2022-10-11</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>285.24</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2318,100 +2318,100 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2022-10-04</t>
+          <t>2022-10-13</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>197.08</v>
+        <v>258.73</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>2022-10-06</t>
+          <t>2022-10-16</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>288.72</v>
+        <v>290.97</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>2022-10-15</t>
+          <t>2022-10-18</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>387.06</v>
+        <v>291.84</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2022-10-17</t>
+          <t>2022-10-19</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>2.75</v>
+        <v>7.38</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>2022-10-18</t>
+          <t>2022-10-20</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>283.61</v>
+        <v>133.95</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
@@ -2423,75 +2423,75 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>2022-10-19</t>
+          <t>2022-10-29</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>91.61</v>
+        <v>407.36</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2022-10-19</t>
+          <t>2022-11-09</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>116.16</v>
+        <v>296.62</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2022-10-21</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>11.56</v>
+        <v>342.56</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>2022-10-21</t>
+          <t>2022-11-19</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>167.42</v>
+        <v>4.48</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>party</t>
         </is>
       </c>
     </row>
@@ -2503,55 +2503,55 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2022-11-01</t>
+          <t>2022-11-20</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>113.17</v>
+        <v>289.78</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>2022-11-08</t>
+          <t>2022-11-22</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>24.66</v>
+        <v>293.36</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>2022-11-11</t>
+          <t>2022-11-22</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>403.72</v>
+        <v>171.64</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
@@ -2563,35 +2563,35 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>2022-11-11</t>
+          <t>2022-11-27</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>358.06</v>
+        <v>121.51</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2022-11-15</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>106.87</v>
+        <v>221.61</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
@@ -2603,155 +2603,155 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>2022-11-22</t>
+          <t>2022-11-28</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>418.38</v>
+        <v>91.78</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2022-11-25</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>66.41</v>
+        <v>368.12</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>2022-11-29</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>140.22</v>
+        <v>23.26</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2022-12-03</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>152.13</v>
+        <v>436.11</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2022-12-08</t>
+          <t>2022-12-06</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>357.23</v>
+        <v>409.51</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>358.07</v>
+        <v>43.35</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2022-12-16</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>374.19</v>
+        <v>89.76000000000001</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2022-12-16</t>
+          <t>2022-12-21</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>169.14</v>
+        <v>373.03</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
@@ -2763,15 +2763,15 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>2022-12-18</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>106.9</v>
+        <v>212.87</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
@@ -2783,62 +2783,62 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2022-12-18</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>304.98</v>
+        <v>41.66</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2022-12-21</t>
+          <t>2022-12-25</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>412.36</v>
+        <v>81.17</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>2022-12-22</t>
+          <t>2022-12-27</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>294.92</v>
+        <v>397.27</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2847,11 +2847,31 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>120.71</v>
+        <v>192.89</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>transport</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Peter James</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>2022-12-30</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>227.23</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>insurance</t>
         </is>
       </c>
     </row>

</xml_diff>